<commit_message>
modified for user defined
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -473,7 +473,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -481,22 +481,22 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="E2" t="n">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="F2" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>7.399999999999999</v>
+        <v>2.899999999999999</v>
       </c>
     </row>
     <row r="3">
@@ -504,30 +504,30 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>fair</t>
+          <t>good</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>74</v>
       </c>
       <c r="E3" t="n">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F3" t="n">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
-        <v>2.899999999999999</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="4">
@@ -535,7 +535,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>49</v>
+        <v>78</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -543,22 +543,22 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="E4" t="n">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="F4" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
       </c>
       <c r="H4" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="I4" t="n">
-        <v>2.899999999999999</v>
+        <v>7.399999999999999</v>
       </c>
     </row>
     <row r="5">
@@ -566,30 +566,30 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>fair</t>
+          <t>good</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="E5" t="n">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="F5" t="n">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1.7</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
       </c>
       <c r="I5" t="n">
-        <v>11.9</v>
+        <v>15.2</v>
       </c>
     </row>
     <row r="6">
@@ -597,30 +597,30 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>fair</t>
+          <t>good</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>98</v>
+        <v>33</v>
       </c>
       <c r="E6" t="n">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="F6" t="n">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="G6" t="n">
-        <v>3.4</v>
+        <v>0</v>
       </c>
       <c r="H6" t="n">
         <v>0</v>
       </c>
       <c r="I6" t="n">
-        <v>18.5</v>
+        <v>11.9</v>
       </c>
     </row>
     <row r="7">
@@ -628,30 +628,30 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>fair</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>65</v>
+        <v>16</v>
       </c>
       <c r="E7" t="n">
-        <v>80</v>
+        <v>50</v>
       </c>
       <c r="F7" t="n">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="G7" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>15.2</v>
+        <v>2.899999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -659,30 +659,30 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>49</v>
+        <v>8</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>fair</t>
+          <t>good</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E8" t="n">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="F8" t="n">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>3.4</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>11.9</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="9">
@@ -690,30 +690,30 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>good</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>97</v>
+      </c>
+      <c r="E9" t="n">
         <v>100</v>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>poor</t>
-        </is>
-      </c>
-      <c r="D9" t="n">
-        <v>73</v>
-      </c>
-      <c r="E9" t="n">
-        <v>60</v>
-      </c>
       <c r="F9" t="n">
-        <v>30</v>
+        <v>50</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>5.100000000000001</v>
       </c>
       <c r="H9" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
-        <v>7.399999999999999</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="10">
@@ -721,30 +721,30 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>fair</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="F10" t="n">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="I10" t="n">
-        <v>11.9</v>
+        <v>-1.600000000000001</v>
       </c>
     </row>
     <row r="11">
@@ -752,7 +752,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -760,22 +760,22 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="E11" t="n">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="F11" t="n">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="G11" t="n">
-        <v>1.7</v>
+        <v>3.4</v>
       </c>
       <c r="H11" t="n">
         <v>0</v>
       </c>
       <c r="I11" t="n">
-        <v>15.2</v>
+        <v>18.5</v>
       </c>
     </row>
     <row r="12">
@@ -783,30 +783,30 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>31</v>
+        <v>78</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>fair</t>
         </is>
       </c>
       <c r="D12" t="n">
+        <v>67</v>
+      </c>
+      <c r="E12" t="n">
         <v>60</v>
       </c>
-      <c r="E12" t="n">
-        <v>80</v>
-      </c>
       <c r="F12" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="G12" t="n">
-        <v>1.7</v>
+        <v>0</v>
       </c>
       <c r="H12" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="I12" t="n">
-        <v>15.2</v>
+        <v>7.399999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -814,15 +814,15 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>good</t>
+          <t>fair</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>29</v>
+        <v>70</v>
       </c>
       <c r="E13" t="n">
         <v>70</v>

</xml_diff>